<commit_message>
XLS MODIFIED - HU
</commit_message>
<xml_diff>
--- a/docs/Historias de USUARIO.xlsx
+++ b/docs/Historias de USUARIO.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\Proyecto FSJS Javiera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\proyectofinal\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58CF4DB-86AB-499F-AE6B-FCD83F157948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94E58B3-696F-4264-890E-FC6A13DDDE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C8424CB0-D5B6-4AE2-9447-D320E95AD064}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C8424CB0-D5B6-4AE2-9447-D320E95AD064}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>HU - 1</t>
   </si>
@@ -94,6 +95,48 @@
   </si>
   <si>
     <t>tabla pedidos/estado</t>
+  </si>
+  <si>
+    <t>HU - 1 Yo como visitante quiero registrarme en el sitio para poder ser un usuario registrado.</t>
+  </si>
+  <si>
+    <t>HU - 2  Yo como usuario registrado, quiero poder acceder al historial de pedidos.</t>
+  </si>
+  <si>
+    <t>HU - 3 Yo como usuario ya registrado puede crear nuevo pedido / solicitud de compra.</t>
+  </si>
+  <si>
+    <t>HU RELACIONADAS AL REGISTRO DE USUARIO Y ACCESO Y SOLICITUD DE COMPRA/PEDIDO</t>
+  </si>
+  <si>
+    <t>HU - 4 Yo como usuario registrado puede leer y listar mis pedidos anteriores.</t>
+  </si>
+  <si>
+    <t>HU - 5 Yo como usuario registrado pueda modificar mis datos personales como por ejemplo "cambiar numero de celular"</t>
+  </si>
+  <si>
+    <t>HU - 6 Yo como usuario registrado puedo acceder a mi información personal almacenada en la DB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU RELACIONADAS AL CRUD y A LA INTERACCION CON LA APP </t>
+  </si>
+  <si>
+    <t>HU RELACIONADAS A LOS PEDIDOS Y PRODUCTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU - 9 Yo como usuario registrado quiero revisar el DETALLE DEL PEDIDO. </t>
+  </si>
+  <si>
+    <t>HU - 11 Yo como usuario registrado, puedo ver el resumen de mi pedido y mandarlo a imprimir y/o mandarlo por email.</t>
+  </si>
+  <si>
+    <t>HU - 7  Yo como usuario registrado quiero ver la informacion del producto, disponibilidad, precio descripcion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU - 8 Yo como usuario registrado, quiero ir agregando estos productos a un PEDIDO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU - 10 Yo como usuario registrado, quiero ver el resumen de mi medido e ingresar la orden de compra/solicitud. </t>
   </si>
 </sst>
 </file>
@@ -453,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21F051F-2DB0-4A56-8EC1-29C273C209E1}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,23 +558,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -539,4 +582,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89DF4E1-6287-45C0-B5CD-106EE4FEB071}">
+  <dimension ref="A3:A25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="109.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>